<commit_message>
Level excel sheet and level manager script
</commit_message>
<xml_diff>
--- a/Normal Pizza for Normal People/Assets/Levels.xlsx
+++ b/Normal Pizza for Normal People/Assets/Levels.xlsx
@@ -59,7 +59,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -68,11 +68,16 @@
     <font>
       <b/>
     </font>
-    <font/>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -88,21 +93,24 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -460,39 +468,39 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>1.0</v>
       </c>
       <c r="B2" s="4">
@@ -501,13 +509,13 @@
       <c r="C2" s="4">
         <v>90.0</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>15.0</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <v>1.0</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="4">
         <v>4.0</v>
       </c>
       <c r="G2" s="4">
@@ -548,7 +556,7 @@
       <c r="Z2" s="5"/>
     </row>
     <row r="3">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>2.0</v>
       </c>
       <c r="B3" s="4">
@@ -557,13 +565,13 @@
       <c r="C3" s="4">
         <v>90.0</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>15.0</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="6">
         <v>1.0</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="4">
         <v>6.0</v>
       </c>
       <c r="G3" s="4">
@@ -604,20 +612,20 @@
       <c r="Z3" s="5"/>
     </row>
     <row r="4">
-      <c r="A4" s="3">
+      <c r="A4" s="4">
         <v>3.0</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="4">
         <v>100.0</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="6">
         <v>20.0</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="6">
         <v>1.0</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="6">
         <v>6.0</v>
       </c>
       <c r="G4" s="4">
@@ -658,20 +666,20 @@
       <c r="Z4" s="5"/>
     </row>
     <row r="5">
-      <c r="A5" s="3">
+      <c r="A5" s="4">
         <v>4.0</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="4">
         <v>100.0</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="6">
         <v>20.0</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="6">
         <v>1.0</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="6">
         <v>8.0</v>
       </c>
       <c r="G5" s="4">
@@ -712,7 +720,7 @@
       <c r="Z5" s="5"/>
     </row>
     <row r="6">
-      <c r="A6" s="3">
+      <c r="A6" s="4">
         <v>5.0</v>
       </c>
       <c r="B6" s="5"/>
@@ -754,7 +762,7 @@
       <c r="Z6" s="5"/>
     </row>
     <row r="7">
-      <c r="A7" s="3">
+      <c r="A7" s="4">
         <v>6.0</v>
       </c>
       <c r="B7" s="5"/>
@@ -796,7 +804,7 @@
       <c r="Z7" s="5"/>
     </row>
     <row r="8">
-      <c r="A8" s="3">
+      <c r="A8" s="4">
         <v>7.0</v>
       </c>
       <c r="B8" s="5"/>
@@ -838,7 +846,7 @@
       <c r="Z8" s="5"/>
     </row>
     <row r="9">
-      <c r="A9" s="3">
+      <c r="A9" s="4">
         <v>8.0</v>
       </c>
       <c r="B9" s="5"/>
@@ -880,7 +888,7 @@
       <c r="Z9" s="5"/>
     </row>
     <row r="10">
-      <c r="A10" s="3">
+      <c r="A10" s="4">
         <v>9.0</v>
       </c>
       <c r="B10" s="5"/>
@@ -922,10 +930,12 @@
       <c r="Z10" s="5"/>
     </row>
     <row r="11">
-      <c r="A11" s="3">
+      <c r="A11" s="4">
         <v>10.0</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="4">
+        <v>69.0</v>
+      </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>

</xml_diff>

<commit_message>
Progress on Level Generation (it does thing)
</commit_message>
<xml_diff>
--- a/Normal Pizza for Normal People/Assets/Levels.xlsx
+++ b/Normal Pizza for Normal People/Assets/Levels.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Normal-Pizza-for-Normal-People\Normal Pizza for Normal People\Assets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6034828A-41D5-4366-B1A5-631B4C3F8B2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -61,160 +70,152 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="4">
     <dxf>
-      <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFACC9FE"/>
+          <bgColor rgb="FFACC9FE"/>
+        </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE8F0FE"/>
+          <bgColor rgb="FFE8F0FE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF5B95F9"/>
           <bgColor rgb="FF5B95F9"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE8F0FE"/>
-          <bgColor rgb="FFE8F0FE"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFACC9FE"/>
-          <bgColor rgb="FFACC9FE"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="4" pivot="0" name="Sheet1-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
-      <tableStyleElement dxfId="4" type="totalRow"/>
+    <tableStyle name="Sheet1-style" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="3"/>
+      <tableStyleElement type="totalRow" dxfId="0"/>
+      <tableStyleElement type="firstRowStripe" dxfId="2"/>
+      <tableStyleElement type="secondRowStripe" dxfId="1"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A1:AA36" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:AA36" headerRowCount="0">
   <tableColumns count="27">
-    <tableColumn name="Column1" id="1"/>
-    <tableColumn name="Column2" id="2"/>
-    <tableColumn name="Column3" id="3"/>
-    <tableColumn name="Column4" id="4"/>
-    <tableColumn name="Column5" id="5"/>
-    <tableColumn name="Column6" id="6"/>
-    <tableColumn name="Column7" id="7"/>
-    <tableColumn name="Column8" id="8"/>
-    <tableColumn name="Column9" id="9"/>
-    <tableColumn name="Column10" id="10"/>
-    <tableColumn name="Column11" id="11"/>
-    <tableColumn name="Column12" id="12"/>
-    <tableColumn name="Column13" id="13"/>
-    <tableColumn name="Column14" id="14"/>
-    <tableColumn name="Column15" id="15"/>
-    <tableColumn name="Column16" id="16"/>
-    <tableColumn name="Column17" id="17"/>
-    <tableColumn name="Column18" id="18"/>
-    <tableColumn name="Column19" id="19"/>
-    <tableColumn name="Column20" id="20"/>
-    <tableColumn name="Column21" id="21"/>
-    <tableColumn name="Column22" id="22"/>
-    <tableColumn name="Column23" id="23"/>
-    <tableColumn name="Column24" id="24"/>
-    <tableColumn name="Column25" id="25"/>
-    <tableColumn name="Column26" id="26"/>
-    <tableColumn name="Column27" id="27"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Column9"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column10"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column11"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Column12"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Column13"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Column14"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Column15"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Column16"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Column17"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Column18"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Column19"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Column20"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Column21"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Column22"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Column23"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Column24"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Column25"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Column26"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Column27"/>
   </tableColumns>
-  <tableStyleInfo name="Sheet1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Sheet1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
@@ -224,7 +225,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -414,42 +415,45 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1.0" ySplit="1.0" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B1" sqref="B1" pane="topRight"/>
-      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
-      <selection activeCell="B2" sqref="B2" pane="bottomRight"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.57"/>
-    <col customWidth="1" min="2" max="2" width="12.0"/>
-    <col customWidth="1" min="3" max="3" width="11.43"/>
-    <col customWidth="1" min="4" max="4" width="16.0"/>
-    <col customWidth="1" min="5" max="5" width="20.0"/>
-    <col customWidth="1" min="6" max="6" width="13.71"/>
-    <col customWidth="1" min="7" max="7" width="13.0"/>
-    <col customWidth="1" min="8" max="8" width="12.86"/>
-    <col customWidth="1" min="9" max="9" width="15.57"/>
-    <col customWidth="1" min="10" max="10" width="11.57"/>
-    <col customWidth="1" min="11" max="11" width="12.86"/>
-    <col customWidth="1" min="12" max="12" width="8.57"/>
-    <col customWidth="1" min="13" max="13" width="10.0"/>
-    <col customWidth="1" min="14" max="14" width="9.0"/>
-    <col customWidth="1" min="15" max="15" width="13.43"/>
+    <col min="1" max="1" width="9.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1"/>
+    <col min="11" max="11" width="12.88671875" customWidth="1"/>
+    <col min="12" max="12" width="8.5546875" customWidth="1"/>
+    <col min="13" max="13" width="10" customWidth="1"/>
+    <col min="14" max="14" width="9" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,33 +512,33 @@
       <c r="Z1" s="3"/>
       <c r="AA1" s="3"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>500.0</v>
+        <v>500</v>
       </c>
       <c r="C2" s="4">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="D2" s="4">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="E2" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G2" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H2" s="4">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I2" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J2" s="4" t="b">
         <v>1</v>
@@ -561,33 +565,33 @@
       <c r="Z2" s="5"/>
       <c r="AA2" s="5"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4">
-        <v>600.0</v>
+        <v>600</v>
       </c>
       <c r="C3" s="4">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="D3" s="4">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="E3" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F3" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G3" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="4">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="I3" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J3" s="4" t="b">
         <v>1</v>
@@ -614,33 +618,33 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="5"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4">
-        <v>600.0</v>
+        <v>600</v>
       </c>
       <c r="C4" s="4">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D4" s="6">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="E4" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F4" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="6">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="I4" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="4" t="b">
         <v>1</v>
@@ -667,33 +671,33 @@
       <c r="Z4" s="5"/>
       <c r="AA4" s="5"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4">
-        <v>800.0</v>
+        <v>800</v>
       </c>
       <c r="C5" s="4">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D5" s="6">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="E5" s="4">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F5" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G5" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="6">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="I5" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J5" s="4" t="b">
         <v>1</v>
@@ -720,33 +724,33 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
-        <v>1000.0</v>
+        <v>1000</v>
       </c>
       <c r="C6" s="4">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D6" s="6">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="E6" s="4">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F6" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G6" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="6">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="I6" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J6" s="4" t="b">
         <v>1</v>
@@ -773,9 +777,9 @@
       <c r="Z6" s="5"/>
       <c r="AA6" s="5"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -810,9 +814,9 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -853,9 +857,9 @@
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -896,9 +900,9 @@
       <c r="Z9" s="5"/>
       <c r="AA9" s="5"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -939,9 +943,9 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="5"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
@@ -982,7 +986,7 @@
       <c r="Z11" s="5"/>
       <c r="AA11" s="5"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1011,7 +1015,7 @@
       <c r="Z12" s="5"/>
       <c r="AA12" s="5"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1040,7 +1044,7 @@
       <c r="Z13" s="5"/>
       <c r="AA13" s="5"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1069,7 +1073,7 @@
       <c r="Z14" s="5"/>
       <c r="AA14" s="5"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1098,7 +1102,7 @@
       <c r="Z15" s="5"/>
       <c r="AA15" s="5"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1127,7 +1131,7 @@
       <c r="Z16" s="5"/>
       <c r="AA16" s="5"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1156,7 +1160,7 @@
       <c r="Z17" s="5"/>
       <c r="AA17" s="5"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1185,7 +1189,7 @@
       <c r="Z18" s="5"/>
       <c r="AA18" s="5"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1214,7 +1218,7 @@
       <c r="Z19" s="5"/>
       <c r="AA19" s="5"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1243,7 +1247,7 @@
       <c r="Z20" s="5"/>
       <c r="AA20" s="5"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1272,7 +1276,7 @@
       <c r="Z21" s="5"/>
       <c r="AA21" s="5"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1301,7 +1305,7 @@
       <c r="Z22" s="5"/>
       <c r="AA22" s="5"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1330,7 +1334,7 @@
       <c r="Z23" s="5"/>
       <c r="AA23" s="5"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1359,7 +1363,7 @@
       <c r="Z24" s="5"/>
       <c r="AA24" s="5"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1388,7 +1392,7 @@
       <c r="Z25" s="5"/>
       <c r="AA25" s="5"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1417,7 +1421,7 @@
       <c r="Z26" s="5"/>
       <c r="AA26" s="5"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1446,7 +1450,7 @@
       <c r="Z27" s="5"/>
       <c r="AA27" s="5"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1475,7 +1479,7 @@
       <c r="Z28" s="5"/>
       <c r="AA28" s="5"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1504,7 +1508,7 @@
       <c r="Z29" s="5"/>
       <c r="AA29" s="5"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1533,7 +1537,7 @@
       <c r="Z30" s="5"/>
       <c r="AA30" s="5"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1562,7 +1566,7 @@
       <c r="Z31" s="5"/>
       <c r="AA31" s="5"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -1591,7 +1595,7 @@
       <c r="Z32" s="5"/>
       <c r="AA32" s="5"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -1620,7 +1624,7 @@
       <c r="Z33" s="5"/>
       <c r="AA33" s="5"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -1649,7 +1653,7 @@
       <c r="Z34" s="5"/>
       <c r="AA34" s="5"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -1678,7 +1682,7 @@
       <c r="Z35" s="5"/>
       <c r="AA35" s="5"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1708,26 +1712,26 @@
       <c r="AA36" s="5"/>
     </row>
   </sheetData>
-  <dataValidations>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="B2:C36">
-      <formula1>0.0</formula1>
+  <dataValidations count="4">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="B2:C36" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between 0 and 2. 0 is low, 1 is mid, 2 is high" sqref="I2:I36">
-      <formula1>0.0</formula1>
-      <formula2>2.0</formula2>
+    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between 0 and 2. 0 is low, 1 is mid, 2 is high" sqref="I2:I36" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>0</formula1>
+      <formula2>2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between 0 and 2" sqref="F2:F36">
-      <formula1>0.0</formula1>
-      <formula2>2.0</formula2>
+    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between 0 and 2" sqref="F2:F36" xr:uid="{00000000-0002-0000-0000-000002000000}">
+      <formula1>0</formula1>
+      <formula2>2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between 0 and 3" sqref="E2:E36">
-      <formula1>0.0</formula1>
-      <formula2>3.0</formula2>
+    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between 0 and 3" sqref="E2:E36" xr:uid="{00000000-0002-0000-0000-000003000000}">
+      <formula1>0</formula1>
+      <formula2>3</formula2>
     </dataValidation>
   </dataValidations>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixing Issues with Materials, Shaders, and Difficulty
Fixed issues with toppings not having the right grab material assigned. Fixed the hologram shader to not use screenspace + also rotated the topping labels to scroll down without screenspace. Adjusted difficulty of days in spreadsheet.
</commit_message>
<xml_diff>
--- a/Normal Pizza for Normal People/Assets/Levels.xlsx
+++ b/Normal Pizza for Normal People/Assets/Levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Normal-Pizza-for-Normal-People\Normal Pizza for Normal People\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789821DF-8635-40C2-94FD-E837C8D494FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B936E27F-D213-4F80-A0F3-FBE04EAAABAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -431,10 +431,10 @@
   <dimension ref="A1:AA36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomRight" activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -443,11 +443,11 @@
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="11.44140625" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
     <col min="10" max="10" width="11.5546875" customWidth="1"/>
     <col min="11" max="11" width="12.88671875" customWidth="1"/>
     <col min="12" max="12" width="8.5546875" customWidth="1"/>
@@ -522,7 +522,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="C2" s="4">
         <v>90</v>
@@ -578,7 +578,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="C3" s="4">
         <v>90</v>
@@ -634,7 +634,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4">
-        <v>600</v>
+        <v>550</v>
       </c>
       <c r="C4" s="4">
         <v>100</v>
@@ -690,7 +690,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="C5" s="4">
         <v>100</v>
@@ -705,7 +705,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5" s="6">
         <v>8</v>
@@ -746,7 +746,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="C6" s="4">
         <v>100</v>
@@ -761,7 +761,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H6" s="6">
         <v>10</v>
@@ -798,9 +798,7 @@
       <c r="AA6" s="5"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
+      <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -809,27 +807,13 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="L7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="M7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="N7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="O7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="P7" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
       <c r="X7" s="5"/>
@@ -838,9 +822,7 @@
       <c r="AA7" s="5"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
+      <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -849,27 +831,13 @@
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="M8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="N8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="O8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="P8" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
@@ -883,9 +851,7 @@
       <c r="AA8" s="5"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
+      <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -894,27 +860,13 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="L9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="M9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="N9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="O9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="P9" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
@@ -928,9 +880,7 @@
       <c r="AA9" s="5"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
+      <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -939,27 +889,13 @@
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
-      <c r="J10" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="L10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="M10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="N10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="O10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="P10" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
       <c r="S10" s="5"/>
@@ -973,9 +909,7 @@
       <c r="AA10" s="5"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
+      <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -984,27 +918,13 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="L11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="M11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="N11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="O11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="P11" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
       <c r="S11" s="5"/>

</xml_diff>

<commit_message>
Fixed Customer Lines not Working + Test Level Window
</commit_message>
<xml_diff>
--- a/Normal Pizza for Normal People/Assets/Levels.xlsx
+++ b/Normal Pizza for Normal People/Assets/Levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Normal-Pizza-for-Normal-People\Normal Pizza for Normal People\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B936E27F-D213-4F80-A0F3-FBE04EAAABAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2FA401E-311E-4B54-9F80-2E0D05B83D0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>DayNum</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>ToppingRange</t>
+  </si>
+  <si>
+    <t>Cheeses</t>
   </si>
 </sst>
 </file>
@@ -431,10 +434,10 @@
   <dimension ref="A1:AA36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P12" sqref="P12"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -505,7 +508,9 @@
       <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="3"/>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="R1" s="3"/>
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
@@ -566,6 +571,9 @@
       <c r="P2" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
       <c r="V2" s="5"/>
       <c r="W2" s="5"/>
       <c r="X2" s="5"/>
@@ -622,6 +630,9 @@
       <c r="P3" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
       <c r="V3" s="5"/>
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
@@ -678,6 +689,9 @@
       <c r="P4" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
@@ -734,6 +748,9 @@
       <c r="P5" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
       <c r="V5" s="5"/>
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
@@ -764,7 +781,7 @@
         <v>3</v>
       </c>
       <c r="H6" s="6">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I6" s="4">
         <v>0</v>
@@ -788,6 +805,9 @@
         <v>1</v>
       </c>
       <c r="P6" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q6">
         <v>0</v>
       </c>
       <c r="V6" s="5"/>
@@ -1460,23 +1480,57 @@
       <c r="AA29" s="5"/>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
+      <c r="A30" s="5">
+        <v>999</v>
+      </c>
+      <c r="B30" s="5">
+        <v>1</v>
+      </c>
+      <c r="C30" s="5">
+        <v>200</v>
+      </c>
+      <c r="D30" s="5">
+        <v>50</v>
+      </c>
+      <c r="E30" s="5">
+        <v>3</v>
+      </c>
+      <c r="F30" s="5">
+        <v>2</v>
+      </c>
+      <c r="G30" s="5">
+        <v>1</v>
+      </c>
+      <c r="H30" s="5">
+        <v>9</v>
+      </c>
+      <c r="I30" s="5">
+        <v>1</v>
+      </c>
+      <c r="J30" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="L30" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="M30" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="N30" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="O30" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="P30" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="5">
+        <v>3</v>
+      </c>
       <c r="R30" s="5"/>
       <c r="S30" s="5"/>
       <c r="T30" s="5"/>
@@ -1604,35 +1658,6 @@
       <c r="Z34" s="5"/>
       <c r="AA34" s="5"/>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="7"/>
-      <c r="M35" s="7"/>
-      <c r="N35" s="7"/>
-      <c r="O35" s="7"/>
-      <c r="P35" s="5"/>
-      <c r="Q35" s="5"/>
-      <c r="R35" s="5"/>
-      <c r="S35" s="5"/>
-      <c r="T35" s="5"/>
-      <c r="U35" s="5"/>
-      <c r="V35" s="5"/>
-      <c r="W35" s="5"/>
-      <c r="X35" s="5"/>
-      <c r="Y35" s="5"/>
-      <c r="Z35" s="5"/>
-      <c r="AA35" s="5"/>
-    </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
@@ -1663,21 +1688,29 @@
       <c r="AA36" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="B2:C36" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="6">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="B36:C36 B2:C34" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between 0 and 2. 0 is low, 1 is mid, 2 is high" sqref="I2:I36" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between 0 and 2. 0 is low, 1 is mid, 2 is high" sqref="I36 I2:I34" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>0</formula1>
       <formula2>2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between 0 and 2" sqref="F2:F36" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between 0 and 2" sqref="F36 F2:F34" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>0</formula1>
       <formula2>2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between 0 and 3" sqref="E2:E36" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between 0 and 3" sqref="E36 E2:E34" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>0</formula1>
       <formula2>3</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q36:Q1048576 Q2:Q34" xr:uid="{2491BBF9-BB54-4852-B95D-25CCEDA9E525}">
+      <formula1>0</formula1>
+      <formula2>3</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576 G2:G1048576" xr:uid="{1BE3871E-2B66-44DC-86F7-85D9D49E4F59}">
+      <formula1>1</formula1>
+      <formula2>9</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Cheese Press to Levels
</commit_message>
<xml_diff>
--- a/Normal Pizza for Normal People/Assets/Levels.xlsx
+++ b/Normal Pizza for Normal People/Assets/Levels.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Normal-Pizza-for-Normal-People\Normal Pizza for Normal People\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E263102E-4FB0-4816-9D43-F00E99EC4FDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04637223-CADD-4FA2-922E-902522FFA4B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -476,10 +476,10 @@
   <dimension ref="A1:AC36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C29" sqref="C29"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -692,10 +692,10 @@
         <v>0</v>
       </c>
       <c r="R3" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
@@ -757,10 +757,10 @@
         <v>0</v>
       </c>
       <c r="R4" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
@@ -822,10 +822,10 @@
         <v>0</v>
       </c>
       <c r="R5" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
@@ -887,10 +887,10 @@
         <v>1</v>
       </c>
       <c r="R6" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
@@ -1852,7 +1852,7 @@
       <formula1>0</formula1>
       <formula2>3</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576 I2:I1048576" xr:uid="{1BE3871E-2B66-44DC-86F7-85D9D49E4F59}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:J1048576" xr:uid="{1BE3871E-2B66-44DC-86F7-85D9D49E4F59}">
       <formula1>1</formula1>
       <formula2>9</formula2>
     </dataValidation>

</xml_diff>